<commit_message>
add login cookie and graphanalysis model testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/data/login-test.xlsx
+++ b/src/main/resources/data/login-test.xlsx
@@ -14,21 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
   <si>
-    <t>name</t>
+    <t>params</t>
   </si>
   <si>
-    <t>password</t>
+    <t>expectCode</t>
   </si>
   <si>
-    <t>expect_code</t>
+    <t>expectMessage</t>
   </si>
   <si>
-    <t>expect_message</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>{"name":"test","password":123}</t>
   </si>
   <si>
     <t>100</t>
@@ -42,9 +39,6 @@
   <si>
     <t>未经授权访问! 账号或密码不正确!</t>
   </si>
-  <si>
-    <t>参数错误! 密码不能为空</t>
-  </si>
 </sst>
 </file>
 
@@ -52,9 +46,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -99,10 +93,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -115,6 +132,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
@@ -122,8 +147,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -137,6 +163,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
@@ -144,9 +178,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,6 +194,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -174,59 +221,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -261,37 +255,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,31 +357,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,19 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,80 +427,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -474,21 +468,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -508,21 +487,6 @@
       </left>
       <right style="thin">
         <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -596,6 +560,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -607,17 +591,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,156 +609,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -795,7 +759,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -811,37 +775,28 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2009,251 +1964,209 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="3" width="16.3482142857143" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.2232142857143" style="1" customWidth="1"/>
-    <col min="5" max="16383" width="16.3482142857143" style="1" customWidth="1"/>
-    <col min="16384" max="16384" width="16.3303571428571" style="1"/>
+    <col min="1" max="2" width="16.3482142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.2232142857143" style="1" customWidth="1"/>
+    <col min="4" max="16382" width="16.3482142857143" style="1" customWidth="1"/>
+    <col min="16383" max="16384" width="16.3303571428571" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1" spans="1:7">
+    <row r="1" ht="20.25" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="5">
-        <v>123</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1" spans="1:6">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" ht="20.05" customHeight="1" spans="1:7">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="9">
-        <v>111</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1" spans="1:7">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14">
-        <v>201</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+    <row r="4" ht="20.05" customHeight="1" spans="1:6">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1" spans="1:7">
+    <row r="5" ht="20.05" customHeight="1" spans="1:6">
       <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1" spans="1:7">
+    <row r="6" ht="20.05" customHeight="1" spans="1:6">
       <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1" spans="1:7">
+    <row r="7" ht="20.05" customHeight="1" spans="1:6">
       <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1" spans="1:7">
+    <row r="8" ht="20.05" customHeight="1" spans="1:6">
       <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
-    <row r="9" ht="20.05" customHeight="1" spans="1:7">
+    <row r="9" ht="20.05" customHeight="1" spans="1:6">
       <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
-    <row r="10" ht="20.05" customHeight="1" spans="1:7">
+    <row r="10" ht="20.05" customHeight="1" spans="1:6">
       <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
-    <row r="11" ht="20.05" customHeight="1" spans="1:7">
+    <row r="11" ht="20.05" customHeight="1" spans="1:6">
       <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
-    <row r="12" ht="20.05" customHeight="1" spans="1:7">
+    <row r="12" ht="20.05" customHeight="1" spans="1:6">
       <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
-    <row r="13" ht="20.05" customHeight="1" spans="1:7">
+    <row r="13" ht="20.05" customHeight="1" spans="1:6">
       <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
-    <row r="14" ht="20.05" customHeight="1" spans="1:7">
+    <row r="14" ht="20.05" customHeight="1" spans="1:6">
       <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
-    <row r="15" ht="20.05" customHeight="1" spans="1:7">
+    <row r="15" ht="20.05" customHeight="1" spans="1:6">
       <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
-    <row r="16" ht="20.05" customHeight="1" spans="1:7">
+    <row r="16" ht="20.05" customHeight="1" spans="1:6">
       <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
-    <row r="17" ht="20.05" customHeight="1" spans="1:7">
+    <row r="17" ht="20.05" customHeight="1" spans="1:6">
       <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
-    <row r="18" ht="20.05" customHeight="1" spans="1:7">
+    <row r="18" ht="20.05" customHeight="1" spans="1:6">
       <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
-    <row r="19" ht="20.05" customHeight="1" spans="1:7">
+    <row r="19" ht="20.05" customHeight="1" spans="1:6">
       <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
-    <row r="20" ht="20.05" customHeight="1" spans="1:7">
+    <row r="20" ht="20.05" customHeight="1" spans="1:6">
       <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
-    <row r="21" ht="20.05" customHeight="1" spans="1:7">
+    <row r="21" ht="20.05" customHeight="1" spans="1:6">
       <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1" spans="1:7">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277777777777778" footer="0.277777777777778"/>

</xml_diff>